<commit_message>
creación de python notebook para gestionar todos los csv
</commit_message>
<xml_diff>
--- a/DesarrolloPy/NormasArregloCSV.xlsx
+++ b/DesarrolloPy/NormasArregloCSV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11586379-9121-4CFB-AC51-E8057FCCCF67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B5A6A4-8DF7-4AAE-B022-F028DFC414C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{591C895C-A150-40E8-91FB-92FBB0EAF9F6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>GENERAL DATA - GD</t>
   </si>
@@ -168,13 +168,85 @@
   </si>
   <si>
     <t>Camp_MovementReason</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>NAUTIA_1_0_Entities_Interview_results.csv</t>
+  </si>
+  <si>
+    <t>Camp_Integration</t>
+  </si>
+  <si>
+    <t>Camp_NaturalHazard</t>
+  </si>
+  <si>
+    <t>"Enviormental_Issues:Risk:Risk_Flood"</t>
+  </si>
+  <si>
+    <t>"Enviormental_Issues:Deforestation"</t>
+  </si>
+  <si>
+    <t>Camp_LocalVegetation</t>
+  </si>
+  <si>
+    <t>"Enviormental_Issues:Native_Plant"</t>
+  </si>
+  <si>
+    <t>"Enviormental_Issues:Native_Crops"</t>
+  </si>
+  <si>
+    <t>Camp_LocalCrop</t>
+  </si>
+  <si>
+    <t>Camp_ClimaticRegion</t>
+  </si>
+  <si>
+    <t>inconsistencia CSV</t>
+  </si>
+  <si>
+    <t>"Tropical (Write one: Af, Aw or Am)"</t>
+  </si>
+  <si>
+    <t>"Continental (Write one: Dfa, Bwa, Dsa or Dfb, Dwb, Dsb)"</t>
+  </si>
+  <si>
+    <t>metodo específico</t>
+  </si>
+  <si>
+    <t>método específico</t>
+  </si>
+  <si>
+    <t>"Max (ºC)"</t>
+  </si>
+  <si>
+    <t>"Relative humidity (%)"</t>
+  </si>
+  <si>
+    <t>"Wind speed"</t>
+  </si>
+  <si>
+    <t>"Max (mm)"</t>
+  </si>
+  <si>
+    <t>Camp_EnergySource</t>
+  </si>
+  <si>
+    <t>2 csv distintos</t>
+  </si>
+  <si>
+    <t>"Fuel_Cost Main_Fuel"</t>
+  </si>
+  <si>
+    <t>Rellenar un formulario para ver"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +270,14 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,12 +333,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,17 +656,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B497A2A-6133-4211-9CA4-B1DE4BEF4C7C}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
@@ -940,10 +1021,18 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="B25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -960,17 +1049,27 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B27" s="3"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="B27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -980,17 +1079,27 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B29" s="3"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="B29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B30" s="3"/>
+      <c r="B30" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1000,17 +1109,27 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B31" s="3"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1020,29 +1139,55 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B33" s="3"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="B33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="D34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="3"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="B35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1050,7 +1195,9 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>

</xml_diff>

<commit_message>
nueva visualizacion de csvs
</commit_message>
<xml_diff>
--- a/DesarrolloPy/NormasArregloCSV.xlsx
+++ b/DesarrolloPy/NormasArregloCSV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D15FDC4-BE9D-4179-84C6-87C540F47B39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AB0F54-7E73-4D4E-8AED-481D17A1F1D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{591C895C-A150-40E8-91FB-92FBB0EAF9F6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
   <si>
     <t>GENERAL DATA - GD</t>
   </si>
@@ -268,6 +268,108 @@
   </si>
   <si>
     <t>pendiente de confirmación</t>
+  </si>
+  <si>
+    <t>Socio Económicos</t>
+  </si>
+  <si>
+    <t>SE_Population</t>
+  </si>
+  <si>
+    <t>NAUTIA_1_0_Entities_Interview_results.csv
+NAUTIA_1_0_General_form_v3_results.csv</t>
+  </si>
+  <si>
+    <t>NECESARIO METODO ESPECIAL
+ (Hombres + Mujeres)</t>
+  </si>
+  <si>
+    <t>NAUTIA_1_0_General_form_v3_results.csv</t>
+  </si>
+  <si>
+    <t>"Social_information:Disability"</t>
+  </si>
+  <si>
+    <t>SE_HouseHold_Composition</t>
+  </si>
+  <si>
+    <t>"General:Old_women"</t>
+  </si>
+  <si>
+    <t>"General:Children"</t>
+  </si>
+  <si>
+    <t>Necesario metodo especial y reordenacion</t>
+  </si>
+  <si>
+    <t>NAUTIA_1_0_Survey_household_v6_results.csv</t>
+  </si>
+  <si>
+    <t>SE_PersonalHygiene</t>
+  </si>
+  <si>
+    <t>"Sanitation:Personal_hygiene"</t>
+  </si>
+  <si>
+    <t>SE_CleaningMaterial</t>
+  </si>
+  <si>
+    <t>"Sanitation:Excreta"</t>
+  </si>
+  <si>
+    <t>SE_SafetyPlace</t>
+  </si>
+  <si>
+    <t>"Feel_Safe:Street_morning"</t>
+  </si>
+  <si>
+    <t>"Feel_Safe:Firewood_collection_001"</t>
+  </si>
+  <si>
+    <t>NAUTIA_1_0_Women_Focus_Group2_results.csv</t>
+  </si>
+  <si>
+    <t>SE_ConflictArea</t>
+  </si>
+  <si>
+    <t>"Trouble_Spots"</t>
+  </si>
+  <si>
+    <t>Revisar respuesta</t>
+  </si>
+  <si>
+    <t>"Settlement_security:secur_committees"</t>
+  </si>
+  <si>
+    <t>NAUTIA_1_0_Local_leaders_v3_results.csv
+NAUTIA_1_0_Entities_Interview_results.csv</t>
+  </si>
+  <si>
+    <t>"Women_Patrol"</t>
+  </si>
+  <si>
+    <t>SE_SafetyCommitte</t>
+  </si>
+  <si>
+    <t>SE_SafetyLatrines</t>
+  </si>
+  <si>
+    <t>NAUTIA_V1_0_Sanitation_Infrastructre_results.csv</t>
+  </si>
+  <si>
+    <t>"Public_Latrines:Sex_segregated"</t>
+  </si>
+  <si>
+    <t>"Public_Latrines:Lighting"</t>
+  </si>
+  <si>
+    <t>SE_Economy</t>
+  </si>
+  <si>
+    <t>"Costs:cost_basic_basket"</t>
+  </si>
+  <si>
+    <t>SE_IncomeType</t>
   </si>
 </sst>
 </file>
@@ -685,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B497A2A-6133-4211-9CA4-B1DE4BEF4C7C}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,7 +800,7 @@
     <col min="3" max="3" width="37.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1169,7 +1271,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B33" s="3" t="s">
         <v>55</v>
       </c>
@@ -1195,7 +1297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="1"/>
       <c r="D34" s="5" t="s">
@@ -1209,7 +1311,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>65</v>
       </c>
@@ -1229,7 +1331,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
         <v>66</v>
       </c>
@@ -1247,7 +1349,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B37" s="3" t="s">
         <v>72</v>
       </c>
@@ -1265,7 +1367,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1275,7 +1377,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
@@ -1293,7 +1395,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B40" s="4" t="s">
         <v>77</v>
       </c>
@@ -1305,6 +1407,425 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B45" s="4"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B47" s="3"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B49" s="4"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B50" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B51" s="4"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B52" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B53" s="4"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B54" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B55" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="2:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="B56" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B57" s="3"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B58" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B59" s="3"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B60" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B61" s="4"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B62" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B63" s="3"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B64" s="3"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B65" s="3"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B66" s="3"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B67" s="4"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B68" s="3"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B69" s="3"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B70" s="3"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B71" s="3"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B72" s="3"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B73" s="4"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
avance en la T
</commit_message>
<xml_diff>
--- a/DesarrolloPy/NormasArregloCSV.xlsx
+++ b/DesarrolloPy/NormasArregloCSV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35D685E-FE52-411D-A4E7-54FA0470B1A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BD97E0-A3EA-45D3-85C7-E88BEBA3F807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{591C895C-A150-40E8-91FB-92FBB0EAF9F6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="112">
   <si>
     <t>GENERAL DATA - GD</t>
   </si>
@@ -370,13 +370,16 @@
   </si>
   <si>
     <t>SE_IncomeType</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +414,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -472,6 +483,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B497A2A-6133-4211-9CA4-B1DE4BEF4C7C}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -837,6 +851,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -859,9 +876,7 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>